<commit_message>
Added control systeem simulations
</commit_message>
<xml_diff>
--- a/OENG1118/Normalization scores ReCiPe 2016.xlsx
+++ b/OENG1118/Normalization scores ReCiPe 2016.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adityaaaap/Desktop/RMIT Master of Mechatronics and Robotics Engineering/sem-2-mc256/OENG1118/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EBE248-9028-8342-93C8-BAB1057EC29E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A61E889-1089-DB4C-B536-F60A112EB214}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final normalization scores" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -4677,7 +4677,7 @@
   <dimension ref="A1:K62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -4753,7 +4753,7 @@
         <v>10757.058940165556</v>
       </c>
       <c r="D4" s="4">
-        <v>7990.407652952963</v>
+        <v>7990.4076529529602</v>
       </c>
       <c r="E4" s="4">
         <v>5797.6041066401167</v>
@@ -4766,7 +4766,7 @@
         <v>8.7347318594144273E-4</v>
       </c>
       <c r="I4" s="6">
-        <v>7.415098301940347E-3</v>
+        <v>7.4150983019403496E-3</v>
       </c>
       <c r="J4" s="6">
         <v>7.2470051333001495E-2</v>
@@ -5029,7 +5029,7 @@
         <v>5.7227553561680741E-6</v>
       </c>
       <c r="I14" s="6">
-        <v>2.2373141428268291E-5</v>
+        <v>2.2373141428268301E-5</v>
       </c>
       <c r="J14" s="6">
         <v>1.4494010266600301E-4</v>
@@ -5232,7 +5232,7 @@
         <v>1.5597735463240051E-10</v>
       </c>
       <c r="I22" s="6">
-        <v>6.112661854509017E-10</v>
+        <v>6.1126618545090201E-10</v>
       </c>
       <c r="J22" s="6">
         <v>3.9539660007285609E-9</v>
@@ -5481,9 +5481,7 @@
       <c r="H33" s="10">
         <v>291.35213967771415</v>
       </c>
-      <c r="I33" s="10">
-        <v>291.35213967771415</v>
-      </c>
+      <c r="I33" s="10"/>
       <c r="J33" s="10">
         <v>291.35213967771415</v>
       </c>

</xml_diff>